<commit_message>
Feat: Nuevo estilo para el Login
</commit_message>
<xml_diff>
--- a/app/data/registros_pos.xlsx
+++ b/app/data/registros_pos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
   <si>
     <t>Nombre</t>
   </si>
@@ -50,6 +50,15 @@
   </si>
   <si>
     <t>VENTA - ID: V-6BE82862 | Monto: $2,00</t>
+  </si>
+  <si>
+    <t>Americano</t>
+  </si>
+  <si>
+    <t>Latte</t>
+  </si>
+  <si>
+    <t>Capuccino</t>
   </si>
 </sst>
 </file>
@@ -94,7 +103,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -142,6 +151,61 @@
       </c>
       <c r="C4" t="n" s="0">
         <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B5" t="n" s="0">
+        <v>4000.0</v>
+      </c>
+      <c r="C5" t="n" s="0">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B6" t="n" s="0">
+        <v>5000.0</v>
+      </c>
+      <c r="C6" t="n" s="0">
+        <v>80.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B7" t="n" s="0">
+        <v>6000.0</v>
+      </c>
+      <c r="C7" t="n" s="0">
+        <v>70.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="C8" t="n" s="0">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="C9" t="n" s="0">
+        <v>15.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Control de cantidades específicas en carrito de ventas
</commit_message>
<xml_diff>
--- a/app/data/registros_pos.xlsx
+++ b/app/data/registros_pos.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kealm\Documents\Proyectos\SistemaPOS\SistemaPOS\app\data\"/>
     </mc:Choice>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Nombre</t>
   </si>
@@ -58,12 +58,49 @@
   </si>
   <si>
     <t>Capuccino</t>
+  </si>
+  <si>
+    <t>V-99E3C23B</t>
+  </si>
+  <si>
+    <t>2025-08-01 18:44:14</t>
+  </si>
+  <si>
+    <t>Fecha/Hora</t>
+  </si>
+  <si>
+    <t>Operación</t>
+  </si>
+  <si>
+    <t>VENTA - ID: V-99E3C23B | Monto: $8000,00</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>V-745239BB</t>
+  </si>
+  <si>
+    <t>2025-08-01 18:53:47</t>
+  </si>
+  <si>
+    <t>VENTA - ID: V-745239BB | Monto: $12000,00</t>
+  </si>
+  <si>
+    <t>V-58AE91BC</t>
+  </si>
+  <si>
+    <t>2025-08-01 18:54:00</t>
+  </si>
+  <si>
+    <t>VENTA - ID: V-58AE91BC | Monto: $12000,00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -429,7 +466,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
@@ -438,47 +475,47 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B3" s="0">
+        <v>5000</v>
+      </c>
+      <c r="C3" s="0">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B4" s="0">
+        <v>6000</v>
+      </c>
+      <c r="C4" s="0">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="B2">
-        <v>4000</v>
-      </c>
-      <c r="C2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3">
-        <v>5000</v>
-      </c>
-      <c r="C3">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>6000</v>
-      </c>
-      <c r="C4">
-        <v>70</v>
+      <c r="B5" t="n" s="0">
+        <v>4000.0</v>
+      </c>
+      <c r="C5" t="n" s="0">
+        <v>50.0</v>
       </c>
     </row>
   </sheetData>
@@ -488,32 +525,65 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="0">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="C3" t="n" s="0">
+        <v>8000.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C4" t="n" s="0">
+        <v>12000.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C5" t="n" s="0">
+        <v>12000.0</v>
       </c>
     </row>
   </sheetData>
@@ -523,18 +593,42 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Implementar Dashboard completo y corregir error crítico de ventas
</commit_message>
<xml_diff>
--- a/app/data/registros_pos.xlsx
+++ b/app/data/registros_pos.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>Nombre</t>
   </si>
@@ -94,6 +94,45 @@
   </si>
   <si>
     <t>VENTA - ID: V-58AE91BC | Monto: $12000,00</t>
+  </si>
+  <si>
+    <t>Granizado</t>
+  </si>
+  <si>
+    <t>V-376EB348</t>
+  </si>
+  <si>
+    <t>2025-08-01 20:02:27</t>
+  </si>
+  <si>
+    <t>VENTA - ID: V-376EB348 | Monto: $33000,00</t>
+  </si>
+  <si>
+    <t>V-A6E52CA1</t>
+  </si>
+  <si>
+    <t>2025-08-02 00:58:53</t>
+  </si>
+  <si>
+    <t>VENTA - ID: V-A6E52CA1 | Monto: $25000,00</t>
+  </si>
+  <si>
+    <t>V-20BFBEEF</t>
+  </si>
+  <si>
+    <t>2025-08-02 00:59:00</t>
+  </si>
+  <si>
+    <t>VENTA - ID: V-20BFBEEF | Monto: $10000,00</t>
+  </si>
+  <si>
+    <t>V-686EFA3C</t>
+  </si>
+  <si>
+    <t>2025-08-02 00:59:05</t>
+  </si>
+  <si>
+    <t>VENTA - ID: V-686EFA3C | Monto: $60000,00</t>
   </si>
 </sst>
 </file>
@@ -489,22 +528,22 @@
       <c r="A3" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="B3" s="0">
-        <v>5000</v>
-      </c>
-      <c r="C3" s="0">
-        <v>80</v>
+      <c r="B3" s="0" t="n">
+        <v>5000.0</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>44.0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="B4" s="0">
-        <v>6000</v>
-      </c>
-      <c r="C4" s="0">
-        <v>70</v>
+      <c r="B4" s="0" t="n">
+        <v>6000.0</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>67.0</v>
       </c>
     </row>
     <row r="5">
@@ -515,7 +554,7 @@
         <v>4000.0</v>
       </c>
       <c r="C5" t="n" s="0">
-        <v>50.0</v>
+        <v>52.0</v>
       </c>
     </row>
   </sheetData>
@@ -525,7 +564,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -586,6 +625,50 @@
         <v>12000.0</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="C6" t="n" s="0">
+        <v>33000.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C7" t="n" s="0">
+        <v>25000.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="C8" t="n" s="0">
+        <v>10000.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="C9" t="n" s="0">
+        <v>60000.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -593,7 +676,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -631,6 +714,38 @@
         <v>23</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix: auto-merge workflow arreglado
</commit_message>
<xml_diff>
--- a/app/data/registros_pos.xlsx
+++ b/app/data/registros_pos.xlsx
@@ -8,12 +8,13 @@
   <sheets>
     <sheet name="Productos" r:id="rId3" sheetId="1"/>
     <sheet name="Ventas" r:id="rId4" sheetId="2"/>
+    <sheet name="RegistroCaja" r:id="rId5" sheetId="3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Nombre</t>
   </si>
@@ -34,6 +35,42 @@
   </si>
   <si>
     <t>Detalle</t>
+  </si>
+  <si>
+    <t>Americano</t>
+  </si>
+  <si>
+    <t>Expresso</t>
+  </si>
+  <si>
+    <t>Latte</t>
+  </si>
+  <si>
+    <t>Capuccino</t>
+  </si>
+  <si>
+    <t>Granizado de Cafe</t>
+  </si>
+  <si>
+    <t>Cafe Frio</t>
+  </si>
+  <si>
+    <t>Iced Latte</t>
+  </si>
+  <si>
+    <t>ID Venta</t>
+  </si>
+  <si>
+    <t>Fecha/Hora</t>
+  </si>
+  <si>
+    <t>V-164B0BBD</t>
+  </si>
+  <si>
+    <t>2025-08-02 02:05:55</t>
+  </si>
+  <si>
+    <t>VENTA - ID: V-164B0BBD | Monto: $66000,00</t>
   </si>
 </sst>
 </file>
@@ -78,7 +115,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -95,6 +132,83 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B2" t="n" s="0">
+        <v>4000.0</v>
+      </c>
+      <c r="C2" t="n" s="0">
+        <v>37.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B3" t="n" s="0">
+        <v>3500.0</v>
+      </c>
+      <c r="C3" t="n" s="0">
+        <v>48.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B4" t="n" s="0">
+        <v>5000.0</v>
+      </c>
+      <c r="C4" t="n" s="0">
+        <v>74.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B5" t="n" s="0">
+        <v>6000.0</v>
+      </c>
+      <c r="C5" t="n" s="0">
+        <v>65.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B6" t="n" s="0">
+        <v>12000.0</v>
+      </c>
+      <c r="C6" t="n" s="0">
+        <v>21.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B7" t="n" s="0">
+        <v>6000.0</v>
+      </c>
+      <c r="C7" t="n" s="0">
+        <v>35.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B8" t="n" s="0">
+        <v>7000.0</v>
+      </c>
+      <c r="C8" t="n" s="0">
+        <v>51.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -102,7 +216,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -110,16 +224,45 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="D1" t="s" s="0">
-        <v>6</v>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C2" t="n" s="0">
+        <v>66000.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>